<commit_message>
update with admin page
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -4,7 +4,6 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="Contacts1" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -398,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -408,88 +407,50 @@
         <v>Timestamp</v>
       </c>
       <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Time</v>
+      </c>
+      <c r="D1" t="str">
         <v>Name</v>
       </c>
-      <c r="C1" t="str">
+      <c r="E1" t="str">
         <v>Email</v>
       </c>
-      <c r="D1" t="str">
+      <c r="F1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="G1" t="str">
         <v>Message</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-07-03T06:29:47.079Z</v>
+        <v>2025-07-03T08:40:26.072Z</v>
       </c>
       <c r="B2" t="str">
-        <v>kunal</v>
+        <v>3/7/2025</v>
       </c>
       <c r="C2" t="str">
+        <v>1:40:26 am</v>
+      </c>
+      <c r="D2" t="str">
+        <v>kunall</v>
+      </c>
+      <c r="E2" t="str">
         <v>kunaldutt69@gmail.com</v>
       </c>
-      <c r="D2" t="str">
-        <v>please take down</v>
+      <c r="F2" t="str">
+        <v>9328068456</v>
+      </c>
+      <c r="G2" t="str">
+        <v>please takedown</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Timestamp</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Email</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Message</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2025-07-03T06:29:47.079Z</v>
-      </c>
-      <c r="B2" t="str">
-        <v>kunal</v>
-      </c>
-      <c r="C2" t="str">
-        <v>kunaldutt69@gmail.com</v>
-      </c>
-      <c r="D2" t="str">
-        <v>please take down</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2025-07-03T06:32:49.496Z</v>
-      </c>
-      <c r="B3" t="str">
-        <v>kunal</v>
-      </c>
-      <c r="C3" t="str">
-        <v>kunaldutt69@gmail.com</v>
-      </c>
-      <c r="D3" t="str">
-        <v>please take down</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>